<commit_message>
Lavet frekvenser og andele
</commit_message>
<xml_diff>
--- a/Data/Frekvenser.xlsx
+++ b/Data/Frekvenser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mads\Desktop\Speciale\Kode\Git\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B329C83-5A0D-4353-9337-C0F606517602}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAE3DDB-A7CF-474C-8700-632C840799C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CEFB1AA5-81CE-4E1A-95A3-FAAC0B42E31F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CEFB1AA5-81CE-4E1A-95A3-FAAC0B42E31F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -510,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E3FE51-855A-4744-A6CC-876F371C6BDB}">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,622 +644,1180 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>381</v>
+        <v>527</v>
       </c>
       <c r="B3">
+        <v>560</v>
+      </c>
+      <c r="C3">
         <v>403</v>
       </c>
-      <c r="C3">
-        <v>304</v>
-      </c>
       <c r="D3">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="E3">
-        <v>870</v>
+        <v>1113</v>
       </c>
       <c r="F3">
-        <v>406</v>
+        <v>622</v>
       </c>
       <c r="G3">
-        <v>362</v>
+        <v>482</v>
       </c>
       <c r="H3">
-        <v>374</v>
+        <v>267</v>
       </c>
       <c r="I3">
-        <v>187</v>
+        <v>356</v>
       </c>
       <c r="J3">
-        <v>482</v>
+        <v>785</v>
       </c>
       <c r="K3">
-        <v>194</v>
+        <v>329</v>
       </c>
       <c r="L3">
-        <v>402</v>
+        <v>572</v>
       </c>
       <c r="M3">
-        <v>201</v>
+        <v>263</v>
       </c>
       <c r="N3">
-        <v>317</v>
+        <v>425</v>
       </c>
       <c r="O3">
-        <v>105</v>
+        <v>208</v>
       </c>
       <c r="P3">
-        <v>198</v>
+        <v>245</v>
       </c>
       <c r="Q3">
-        <v>252</v>
+        <v>400</v>
       </c>
       <c r="R3">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="S3">
-        <v>170</v>
+        <v>214</v>
       </c>
       <c r="T3">
-        <v>170</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>554</v>
+        <v>381</v>
       </c>
       <c r="B4">
-        <v>622</v>
+        <v>403</v>
       </c>
       <c r="C4">
+        <v>304</v>
+      </c>
+      <c r="D4">
+        <v>154</v>
+      </c>
+      <c r="E4">
+        <v>870</v>
+      </c>
+      <c r="F4">
         <v>406</v>
       </c>
-      <c r="D4">
-        <v>233</v>
-      </c>
-      <c r="E4">
-        <v>1353</v>
-      </c>
-      <c r="F4">
-        <v>774</v>
-      </c>
       <c r="G4">
-        <v>580</v>
+        <v>362</v>
       </c>
       <c r="H4">
-        <v>548</v>
+        <v>374</v>
       </c>
       <c r="I4">
-        <v>417</v>
+        <v>187</v>
       </c>
       <c r="J4">
-        <v>749</v>
+        <v>482</v>
       </c>
       <c r="K4">
-        <v>575</v>
+        <v>194</v>
       </c>
       <c r="L4">
-        <v>585</v>
+        <v>402</v>
       </c>
       <c r="M4">
-        <v>395</v>
+        <v>201</v>
       </c>
       <c r="N4">
-        <v>424</v>
+        <v>317</v>
       </c>
       <c r="O4">
-        <v>261</v>
+        <v>105</v>
       </c>
       <c r="P4">
-        <v>268</v>
+        <v>198</v>
       </c>
       <c r="Q4">
-        <v>435</v>
+        <v>252</v>
       </c>
       <c r="R4">
-        <v>268</v>
+        <v>157</v>
       </c>
       <c r="S4">
-        <v>250</v>
+        <v>170</v>
       </c>
       <c r="T4">
-        <v>231</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>453</v>
+        <v>184</v>
       </c>
       <c r="B5">
-        <v>482</v>
+        <v>213</v>
       </c>
       <c r="C5">
-        <v>362</v>
+        <v>154</v>
       </c>
       <c r="D5">
+        <v>92</v>
+      </c>
+      <c r="E5">
+        <v>413</v>
+      </c>
+      <c r="F5">
+        <v>233</v>
+      </c>
+      <c r="G5">
         <v>202</v>
       </c>
-      <c r="E5">
-        <v>1084</v>
-      </c>
-      <c r="F5">
-        <v>580</v>
-      </c>
-      <c r="G5">
-        <v>486</v>
-      </c>
       <c r="H5">
-        <v>450</v>
+        <v>200</v>
       </c>
       <c r="I5">
-        <v>313</v>
+        <v>114</v>
       </c>
       <c r="J5">
-        <v>623</v>
+        <v>245</v>
       </c>
       <c r="K5">
-        <v>432</v>
+        <v>132</v>
       </c>
       <c r="L5">
-        <v>497</v>
+        <v>234</v>
       </c>
       <c r="M5">
-        <v>251</v>
+        <v>89</v>
       </c>
       <c r="N5">
-        <v>352</v>
+        <v>155</v>
       </c>
       <c r="O5">
-        <v>206</v>
+        <v>56</v>
       </c>
       <c r="P5">
-        <v>243</v>
+        <v>92</v>
       </c>
       <c r="Q5">
-        <v>329</v>
+        <v>128</v>
       </c>
       <c r="R5">
-        <v>197</v>
+        <v>81</v>
       </c>
       <c r="S5">
-        <v>173</v>
+        <v>79</v>
       </c>
       <c r="T5">
-        <v>162</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>719</v>
+        <v>1376</v>
       </c>
       <c r="B6">
-        <v>785</v>
+        <v>1113</v>
       </c>
       <c r="C6">
-        <v>482</v>
+        <v>870</v>
       </c>
       <c r="D6">
-        <v>245</v>
+        <v>413</v>
       </c>
       <c r="E6">
+        <v>3652</v>
+      </c>
+      <c r="F6">
+        <v>1353</v>
+      </c>
+      <c r="G6">
+        <v>1084</v>
+      </c>
+      <c r="H6">
+        <v>1282</v>
+      </c>
+      <c r="I6">
+        <v>791</v>
+      </c>
+      <c r="J6">
         <v>1796</v>
       </c>
-      <c r="F6">
-        <v>749</v>
-      </c>
-      <c r="G6">
-        <v>623</v>
-      </c>
-      <c r="H6">
-        <v>696</v>
-      </c>
-      <c r="I6">
-        <v>427</v>
-      </c>
-      <c r="J6">
+      <c r="K6">
         <v>756</v>
       </c>
-      <c r="K6">
-        <v>426</v>
-      </c>
       <c r="L6">
-        <v>711</v>
+        <v>1536</v>
       </c>
       <c r="M6">
-        <v>403</v>
+        <v>686</v>
       </c>
       <c r="N6">
-        <v>537</v>
+        <v>879</v>
       </c>
       <c r="O6">
-        <v>256</v>
+        <v>409</v>
       </c>
       <c r="P6">
-        <v>309</v>
+        <v>553</v>
       </c>
       <c r="Q6">
-        <v>471</v>
+        <v>1056</v>
       </c>
       <c r="R6">
-        <v>283</v>
+        <v>513</v>
       </c>
       <c r="S6">
-        <v>240</v>
+        <v>644</v>
       </c>
       <c r="T6">
-        <v>291</v>
+        <v>567</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>260</v>
+        <v>554</v>
       </c>
       <c r="B7">
-        <v>263</v>
+        <v>622</v>
       </c>
       <c r="C7">
-        <v>201</v>
+        <v>406</v>
       </c>
       <c r="D7">
-        <v>89</v>
+        <v>233</v>
       </c>
       <c r="E7">
-        <v>686</v>
+        <v>1353</v>
       </c>
       <c r="F7">
+        <v>774</v>
+      </c>
+      <c r="G7">
+        <v>580</v>
+      </c>
+      <c r="H7">
+        <v>548</v>
+      </c>
+      <c r="I7">
+        <v>417</v>
+      </c>
+      <c r="J7">
+        <v>749</v>
+      </c>
+      <c r="K7">
+        <v>575</v>
+      </c>
+      <c r="L7">
+        <v>585</v>
+      </c>
+      <c r="M7">
         <v>395</v>
       </c>
-      <c r="G7">
-        <v>251</v>
-      </c>
-      <c r="H7">
-        <v>228</v>
-      </c>
-      <c r="I7">
-        <v>168</v>
-      </c>
-      <c r="J7">
-        <v>403</v>
-      </c>
-      <c r="K7">
-        <v>264</v>
-      </c>
-      <c r="L7">
-        <v>321</v>
-      </c>
-      <c r="M7">
-        <v>170</v>
-      </c>
       <c r="N7">
-        <v>180</v>
+        <v>424</v>
       </c>
       <c r="O7">
-        <v>108</v>
+        <v>261</v>
       </c>
       <c r="P7">
-        <v>108</v>
+        <v>268</v>
       </c>
       <c r="Q7">
-        <v>212</v>
+        <v>435</v>
       </c>
       <c r="R7">
-        <v>140</v>
+        <v>268</v>
       </c>
       <c r="S7">
-        <v>161</v>
+        <v>250</v>
       </c>
       <c r="T7">
-        <v>137</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>402</v>
+        <v>453</v>
       </c>
       <c r="B8">
-        <v>425</v>
+        <v>482</v>
       </c>
       <c r="C8">
-        <v>317</v>
+        <v>362</v>
       </c>
       <c r="D8">
-        <v>155</v>
+        <v>202</v>
       </c>
       <c r="E8">
-        <v>879</v>
+        <v>1084</v>
       </c>
       <c r="F8">
-        <v>424</v>
+        <v>580</v>
       </c>
       <c r="G8">
+        <v>486</v>
+      </c>
+      <c r="H8">
+        <v>450</v>
+      </c>
+      <c r="I8">
+        <v>313</v>
+      </c>
+      <c r="J8">
+        <v>623</v>
+      </c>
+      <c r="K8">
+        <v>432</v>
+      </c>
+      <c r="L8">
+        <v>497</v>
+      </c>
+      <c r="M8">
+        <v>251</v>
+      </c>
+      <c r="N8">
         <v>352</v>
       </c>
-      <c r="H8">
-        <v>412</v>
-      </c>
-      <c r="I8">
-        <v>234</v>
-      </c>
-      <c r="J8">
-        <v>537</v>
-      </c>
-      <c r="K8">
-        <v>255</v>
-      </c>
-      <c r="L8">
-        <v>461</v>
-      </c>
-      <c r="M8">
-        <v>180</v>
-      </c>
-      <c r="N8">
-        <v>344</v>
-      </c>
       <c r="O8">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="P8">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="Q8">
-        <v>275</v>
+        <v>329</v>
       </c>
       <c r="R8">
-        <v>161</v>
+        <v>197</v>
       </c>
       <c r="S8">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="T8">
-        <v>179</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>258</v>
+        <v>503</v>
       </c>
       <c r="B9">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="C9">
-        <v>198</v>
+        <v>374</v>
       </c>
       <c r="D9">
-        <v>92</v>
+        <v>200</v>
       </c>
       <c r="E9">
-        <v>553</v>
+        <v>1282</v>
       </c>
       <c r="F9">
-        <v>268</v>
+        <v>548</v>
       </c>
       <c r="G9">
-        <v>243</v>
+        <v>450</v>
       </c>
       <c r="H9">
+        <v>598</v>
+      </c>
+      <c r="I9">
+        <v>331</v>
+      </c>
+      <c r="J9">
+        <v>696</v>
+      </c>
+      <c r="K9">
+        <v>298</v>
+      </c>
+      <c r="L9">
+        <v>593</v>
+      </c>
+      <c r="M9">
+        <v>228</v>
+      </c>
+      <c r="N9">
+        <v>412</v>
+      </c>
+      <c r="O9">
+        <v>171</v>
+      </c>
+      <c r="P9">
         <v>238</v>
       </c>
-      <c r="I9">
-        <v>165</v>
-      </c>
-      <c r="J9">
-        <v>309</v>
-      </c>
-      <c r="K9">
-        <v>140</v>
-      </c>
-      <c r="L9">
-        <v>275</v>
-      </c>
-      <c r="M9">
-        <v>108</v>
-      </c>
-      <c r="N9">
-        <v>231</v>
-      </c>
-      <c r="O9">
-        <v>73</v>
-      </c>
-      <c r="P9">
-        <v>78</v>
-      </c>
       <c r="Q9">
-        <v>159</v>
+        <v>343</v>
       </c>
       <c r="R9">
-        <v>106</v>
+        <v>236</v>
       </c>
       <c r="S9">
-        <v>99</v>
+        <v>214</v>
       </c>
       <c r="T9">
-        <v>96</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>389</v>
+        <v>319</v>
       </c>
       <c r="B10">
-        <v>400</v>
+        <v>356</v>
       </c>
       <c r="C10">
-        <v>252</v>
+        <v>187</v>
       </c>
       <c r="D10">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E10">
-        <v>1056</v>
+        <v>791</v>
       </c>
       <c r="F10">
-        <v>435</v>
+        <v>417</v>
       </c>
       <c r="G10">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="H10">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="I10">
+        <v>214</v>
+      </c>
+      <c r="J10">
+        <v>427</v>
+      </c>
+      <c r="K10">
+        <v>251</v>
+      </c>
+      <c r="L10">
+        <v>336</v>
+      </c>
+      <c r="M10">
+        <v>168</v>
+      </c>
+      <c r="N10">
+        <v>234</v>
+      </c>
+      <c r="O10">
+        <v>140</v>
+      </c>
+      <c r="P10">
+        <v>165</v>
+      </c>
+      <c r="Q10">
         <v>244</v>
       </c>
-      <c r="J10">
-        <v>471</v>
-      </c>
-      <c r="K10">
-        <v>234</v>
-      </c>
-      <c r="L10">
-        <v>449</v>
-      </c>
-      <c r="M10">
-        <v>212</v>
-      </c>
-      <c r="N10">
-        <v>275</v>
-      </c>
-      <c r="O10">
-        <v>134</v>
-      </c>
-      <c r="P10">
-        <v>159</v>
-      </c>
-      <c r="Q10">
-        <v>298</v>
-      </c>
       <c r="R10">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="S10">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="T10">
-        <v>154</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>719</v>
+      </c>
+      <c r="B11">
+        <v>785</v>
+      </c>
+      <c r="C11">
+        <v>482</v>
+      </c>
+      <c r="D11">
         <v>245</v>
       </c>
-      <c r="B11">
-        <v>165</v>
-      </c>
-      <c r="C11">
-        <v>157</v>
-      </c>
-      <c r="D11">
-        <v>81</v>
-      </c>
       <c r="E11">
-        <v>513</v>
+        <v>1796</v>
       </c>
       <c r="F11">
-        <v>268</v>
+        <v>749</v>
       </c>
       <c r="G11">
-        <v>197</v>
+        <v>623</v>
       </c>
       <c r="H11">
-        <v>236</v>
+        <v>696</v>
       </c>
       <c r="I11">
-        <v>130</v>
+        <v>427</v>
       </c>
       <c r="J11">
+        <v>756</v>
+      </c>
+      <c r="K11">
+        <v>426</v>
+      </c>
+      <c r="L11">
+        <v>711</v>
+      </c>
+      <c r="M11">
+        <v>403</v>
+      </c>
+      <c r="N11">
+        <v>537</v>
+      </c>
+      <c r="O11">
+        <v>256</v>
+      </c>
+      <c r="P11">
+        <v>309</v>
+      </c>
+      <c r="Q11">
+        <v>471</v>
+      </c>
+      <c r="R11">
         <v>283</v>
       </c>
-      <c r="K11">
-        <v>150</v>
-      </c>
-      <c r="L11">
-        <v>276</v>
-      </c>
-      <c r="M11">
-        <v>140</v>
-      </c>
-      <c r="N11">
-        <v>161</v>
-      </c>
-      <c r="O11">
-        <v>84</v>
-      </c>
-      <c r="P11">
-        <v>106</v>
-      </c>
-      <c r="Q11">
-        <v>133</v>
-      </c>
-      <c r="R11">
-        <v>82</v>
-      </c>
       <c r="S11">
-        <v>97</v>
+        <v>240</v>
       </c>
       <c r="T11">
-        <v>82</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>336</v>
+      </c>
+      <c r="B12">
+        <v>329</v>
+      </c>
+      <c r="C12">
+        <v>194</v>
+      </c>
+      <c r="D12">
+        <v>132</v>
+      </c>
+      <c r="E12">
+        <v>756</v>
+      </c>
+      <c r="F12">
+        <v>575</v>
+      </c>
+      <c r="G12">
+        <v>432</v>
+      </c>
+      <c r="H12">
+        <v>298</v>
+      </c>
+      <c r="I12">
+        <v>251</v>
+      </c>
+      <c r="J12">
+        <v>426</v>
+      </c>
+      <c r="K12">
+        <v>424</v>
+      </c>
+      <c r="L12">
+        <v>395</v>
+      </c>
+      <c r="M12">
+        <v>264</v>
+      </c>
+      <c r="N12">
+        <v>255</v>
+      </c>
+      <c r="O12">
+        <v>184</v>
+      </c>
+      <c r="P12">
+        <v>140</v>
+      </c>
+      <c r="Q12">
+        <v>234</v>
+      </c>
+      <c r="R12">
+        <v>150</v>
+      </c>
+      <c r="S12">
+        <v>148</v>
+      </c>
+      <c r="T12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>618</v>
+      </c>
+      <c r="B13">
+        <v>572</v>
+      </c>
+      <c r="C13">
+        <v>402</v>
+      </c>
+      <c r="D13">
+        <v>234</v>
+      </c>
+      <c r="E13">
+        <v>1536</v>
+      </c>
+      <c r="F13">
+        <v>585</v>
+      </c>
+      <c r="G13">
+        <v>497</v>
+      </c>
+      <c r="H13">
+        <v>593</v>
+      </c>
+      <c r="I13">
+        <v>336</v>
+      </c>
+      <c r="J13">
+        <v>711</v>
+      </c>
+      <c r="K13">
+        <v>395</v>
+      </c>
+      <c r="L13">
+        <v>710</v>
+      </c>
+      <c r="M13">
+        <v>321</v>
+      </c>
+      <c r="N13">
+        <v>461</v>
+      </c>
+      <c r="O13">
+        <v>224</v>
+      </c>
+      <c r="P13">
+        <v>275</v>
+      </c>
+      <c r="Q13">
+        <v>449</v>
+      </c>
+      <c r="R13">
+        <v>276</v>
+      </c>
+      <c r="S13">
+        <v>274</v>
+      </c>
+      <c r="T13">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>260</v>
+      </c>
+      <c r="B14">
+        <v>263</v>
+      </c>
+      <c r="C14">
+        <v>201</v>
+      </c>
+      <c r="D14">
+        <v>89</v>
+      </c>
+      <c r="E14">
+        <v>686</v>
+      </c>
+      <c r="F14">
+        <v>395</v>
+      </c>
+      <c r="G14">
+        <v>251</v>
+      </c>
+      <c r="H14">
+        <v>228</v>
+      </c>
+      <c r="I14">
+        <v>168</v>
+      </c>
+      <c r="J14">
+        <v>403</v>
+      </c>
+      <c r="K14">
+        <v>264</v>
+      </c>
+      <c r="L14">
+        <v>321</v>
+      </c>
+      <c r="M14">
+        <v>170</v>
+      </c>
+      <c r="N14">
+        <v>180</v>
+      </c>
+      <c r="O14">
+        <v>108</v>
+      </c>
+      <c r="P14">
+        <v>108</v>
+      </c>
+      <c r="Q14">
+        <v>212</v>
+      </c>
+      <c r="R14">
+        <v>140</v>
+      </c>
+      <c r="S14">
+        <v>161</v>
+      </c>
+      <c r="T14">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>402</v>
+      </c>
+      <c r="B15">
+        <v>425</v>
+      </c>
+      <c r="C15">
+        <v>317</v>
+      </c>
+      <c r="D15">
+        <v>155</v>
+      </c>
+      <c r="E15">
+        <v>879</v>
+      </c>
+      <c r="F15">
+        <v>424</v>
+      </c>
+      <c r="G15">
+        <v>352</v>
+      </c>
+      <c r="H15">
+        <v>412</v>
+      </c>
+      <c r="I15">
+        <v>234</v>
+      </c>
+      <c r="J15">
+        <v>537</v>
+      </c>
+      <c r="K15">
+        <v>255</v>
+      </c>
+      <c r="L15">
+        <v>461</v>
+      </c>
+      <c r="M15">
+        <v>180</v>
+      </c>
+      <c r="N15">
+        <v>344</v>
+      </c>
+      <c r="O15">
+        <v>133</v>
+      </c>
+      <c r="P15">
+        <v>231</v>
+      </c>
+      <c r="Q15">
+        <v>275</v>
+      </c>
+      <c r="R15">
+        <v>161</v>
+      </c>
+      <c r="S15">
+        <v>186</v>
+      </c>
+      <c r="T15">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>158</v>
+      </c>
+      <c r="B16">
+        <v>208</v>
+      </c>
+      <c r="C16">
+        <v>105</v>
+      </c>
+      <c r="D16">
+        <v>56</v>
+      </c>
+      <c r="E16">
+        <v>409</v>
+      </c>
+      <c r="F16">
+        <v>261</v>
+      </c>
+      <c r="G16">
+        <v>206</v>
+      </c>
+      <c r="H16">
+        <v>171</v>
+      </c>
+      <c r="I16">
+        <v>140</v>
+      </c>
+      <c r="J16">
+        <v>256</v>
+      </c>
+      <c r="K16">
+        <v>184</v>
+      </c>
+      <c r="L16">
+        <v>224</v>
+      </c>
+      <c r="M16">
+        <v>108</v>
+      </c>
+      <c r="N16">
+        <v>133</v>
+      </c>
+      <c r="O16">
+        <v>74</v>
+      </c>
+      <c r="P16">
+        <v>73</v>
+      </c>
+      <c r="Q16">
+        <v>134</v>
+      </c>
+      <c r="R16">
+        <v>84</v>
+      </c>
+      <c r="S16">
+        <v>72</v>
+      </c>
+      <c r="T16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>258</v>
+      </c>
+      <c r="B17">
+        <v>245</v>
+      </c>
+      <c r="C17">
+        <v>198</v>
+      </c>
+      <c r="D17">
+        <v>92</v>
+      </c>
+      <c r="E17">
+        <v>553</v>
+      </c>
+      <c r="F17">
+        <v>268</v>
+      </c>
+      <c r="G17">
+        <v>243</v>
+      </c>
+      <c r="H17">
+        <v>238</v>
+      </c>
+      <c r="I17">
+        <v>165</v>
+      </c>
+      <c r="J17">
+        <v>309</v>
+      </c>
+      <c r="K17">
+        <v>140</v>
+      </c>
+      <c r="L17">
+        <v>275</v>
+      </c>
+      <c r="M17">
+        <v>108</v>
+      </c>
+      <c r="N17">
+        <v>231</v>
+      </c>
+      <c r="O17">
+        <v>73</v>
+      </c>
+      <c r="P17">
+        <v>78</v>
+      </c>
+      <c r="Q17">
+        <v>159</v>
+      </c>
+      <c r="R17">
+        <v>106</v>
+      </c>
+      <c r="S17">
+        <v>99</v>
+      </c>
+      <c r="T17">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>389</v>
+      </c>
+      <c r="B18">
+        <v>400</v>
+      </c>
+      <c r="C18">
+        <v>252</v>
+      </c>
+      <c r="D18">
+        <v>128</v>
+      </c>
+      <c r="E18">
+        <v>1056</v>
+      </c>
+      <c r="F18">
+        <v>435</v>
+      </c>
+      <c r="G18">
+        <v>329</v>
+      </c>
+      <c r="H18">
+        <v>343</v>
+      </c>
+      <c r="I18">
+        <v>244</v>
+      </c>
+      <c r="J18">
+        <v>471</v>
+      </c>
+      <c r="K18">
+        <v>234</v>
+      </c>
+      <c r="L18">
+        <v>449</v>
+      </c>
+      <c r="M18">
+        <v>212</v>
+      </c>
+      <c r="N18">
+        <v>275</v>
+      </c>
+      <c r="O18">
+        <v>134</v>
+      </c>
+      <c r="P18">
+        <v>159</v>
+      </c>
+      <c r="Q18">
+        <v>298</v>
+      </c>
+      <c r="R18">
+        <v>133</v>
+      </c>
+      <c r="S18">
+        <v>190</v>
+      </c>
+      <c r="T18">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>245</v>
+      </c>
+      <c r="B19">
+        <v>165</v>
+      </c>
+      <c r="C19">
+        <v>157</v>
+      </c>
+      <c r="D19">
+        <v>81</v>
+      </c>
+      <c r="E19">
+        <v>513</v>
+      </c>
+      <c r="F19">
+        <v>268</v>
+      </c>
+      <c r="G19">
+        <v>197</v>
+      </c>
+      <c r="H19">
+        <v>236</v>
+      </c>
+      <c r="I19">
+        <v>130</v>
+      </c>
+      <c r="J19">
+        <v>283</v>
+      </c>
+      <c r="K19">
+        <v>150</v>
+      </c>
+      <c r="L19">
+        <v>276</v>
+      </c>
+      <c r="M19">
+        <v>140</v>
+      </c>
+      <c r="N19">
+        <v>161</v>
+      </c>
+      <c r="O19">
+        <v>84</v>
+      </c>
+      <c r="P19">
+        <v>106</v>
+      </c>
+      <c r="Q19">
+        <v>133</v>
+      </c>
+      <c r="R19">
+        <v>82</v>
+      </c>
+      <c r="S19">
+        <v>97</v>
+      </c>
+      <c r="T19">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>262</v>
       </c>
-      <c r="B12">
+      <c r="B20">
         <v>214</v>
       </c>
-      <c r="C12">
+      <c r="C20">
         <v>170</v>
       </c>
-      <c r="D12">
+      <c r="D20">
         <v>79</v>
       </c>
-      <c r="E12">
+      <c r="E20">
         <v>644</v>
       </c>
-      <c r="F12">
+      <c r="F20">
         <v>250</v>
       </c>
-      <c r="G12">
+      <c r="G20">
         <v>173</v>
       </c>
-      <c r="H12">
+      <c r="H20">
         <v>214</v>
       </c>
-      <c r="I12">
+      <c r="I20">
         <v>153</v>
       </c>
-      <c r="J12">
+      <c r="J20">
         <v>240</v>
       </c>
-      <c r="K12">
+      <c r="K20">
         <v>148</v>
       </c>
-      <c r="L12">
+      <c r="L20">
         <v>274</v>
       </c>
-      <c r="M12">
+      <c r="M20">
         <v>161</v>
       </c>
-      <c r="N12">
+      <c r="N20">
         <v>186</v>
       </c>
-      <c r="O12">
+      <c r="O20">
         <v>72</v>
       </c>
-      <c r="P12">
+      <c r="P20">
         <v>99</v>
       </c>
-      <c r="Q12">
+      <c r="Q20">
         <v>190</v>
       </c>
-      <c r="R12">
+      <c r="R20">
         <v>97</v>
       </c>
-      <c r="S12">
+      <c r="S20">
         <v>114</v>
       </c>
-      <c r="T12">
+      <c r="T20">
         <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>246</v>
+      </c>
+      <c r="B21">
+        <v>229</v>
+      </c>
+      <c r="C21">
+        <v>170</v>
+      </c>
+      <c r="D21">
+        <v>64</v>
+      </c>
+      <c r="E21">
+        <v>567</v>
+      </c>
+      <c r="F21">
+        <v>231</v>
+      </c>
+      <c r="G21">
+        <v>162</v>
+      </c>
+      <c r="H21">
+        <v>168</v>
+      </c>
+      <c r="I21">
+        <v>116</v>
+      </c>
+      <c r="J21">
+        <v>291</v>
+      </c>
+      <c r="K21">
+        <v>35</v>
+      </c>
+      <c r="L21">
+        <v>247</v>
+      </c>
+      <c r="M21">
+        <v>137</v>
+      </c>
+      <c r="N21">
+        <v>179</v>
+      </c>
+      <c r="O21">
+        <v>70</v>
+      </c>
+      <c r="P21">
+        <v>96</v>
+      </c>
+      <c r="Q21">
+        <v>154</v>
+      </c>
+      <c r="R21">
+        <v>82</v>
+      </c>
+      <c r="S21">
+        <v>84</v>
+      </c>
+      <c r="T21">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>